<commit_message>
Added QA Concept Word doc, with initial description
</commit_message>
<xml_diff>
--- a/00_General/QA/QA Data (21_April).xlsx
+++ b/00_General/QA/QA Data (21_April).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\droon\OneDrive\Desktop\UNI\Sem 2\gruppe-15\00_General\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF35A0F-A4B6-4CE7-8E6D-DE824BAF741B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2FC796-2D76-4D44-9949-1AD1B4D3D9F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1252E68F-5E20-402A-B040-0EB0ADF26F11}"/>
   </bookViews>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -437,7 +439,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added data for 27 April, LOC's
</commit_message>
<xml_diff>
--- a/00_General/QA/QA Data (21_April).xlsx
+++ b/00_General/QA/QA Data (21_April).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\droon\OneDrive\Desktop\UNI\Sem 2\gruppe-15\00_General\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2FC796-2D76-4D44-9949-1AD1B4D3D9F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3470E738-194F-4511-AC91-58D250D177F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1252E68F-5E20-402A-B040-0EB0ADF26F11}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{1252E68F-5E20-402A-B040-0EB0ADF26F11}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>GameGraphic.java</t>
   </si>
@@ -69,6 +69,69 @@
   </si>
   <si>
     <t>Total:</t>
+  </si>
+  <si>
+    <t>Card.java</t>
+  </si>
+  <si>
+    <t>CardButton.java</t>
+  </si>
+  <si>
+    <t>CardIcons.java</t>
+  </si>
+  <si>
+    <t>DragDropTest.java</t>
+  </si>
+  <si>
+    <t>Main.java</t>
+  </si>
+  <si>
+    <t>NameTakenException.java</t>
+  </si>
+  <si>
+    <t>NoCommandException.java</t>
+  </si>
+  <si>
+    <t>NotACommandException.java</t>
+  </si>
+  <si>
+    <t>Pile.java</t>
+  </si>
+  <si>
+    <t>Player.java</t>
+  </si>
+  <si>
+    <t>Protocol.java</t>
+  </si>
+  <si>
+    <t>ProtocolExecutorTest.java</t>
+  </si>
+  <si>
+    <t>SBClient.java</t>
+  </si>
+  <si>
+    <t>SBClientListener.java</t>
+  </si>
+  <si>
+    <t>SBListener.java</t>
+  </si>
+  <si>
+    <t>SBLobby.java</t>
+  </si>
+  <si>
+    <t>SBServer.java</t>
+  </si>
+  <si>
+    <t>SBServerListener.java</t>
+  </si>
+  <si>
+    <t>Status.java</t>
+  </si>
+  <si>
+    <t>WindowHandler.java</t>
+  </si>
+  <si>
+    <t>WrapEditorKit.java</t>
   </si>
 </sst>
 </file>
@@ -436,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEAAFE06-F7DA-407D-B53D-9595DF79D1C2}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,6 +838,687 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>46478</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="1">
+        <v>43</v>
+      </c>
+      <c r="C29" s="1">
+        <v>22</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.51162790697674398</v>
+      </c>
+      <c r="E29" s="1">
+        <v>12</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0.27906976744186002</v>
+      </c>
+      <c r="G29" s="1">
+        <v>9</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0.209302325581395</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1">
+        <v>73</v>
+      </c>
+      <c r="C30" s="1">
+        <v>54</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0.73972602739726001</v>
+      </c>
+      <c r="E30" s="1">
+        <v>3</v>
+      </c>
+      <c r="F30" s="1">
+        <v>4.1095890410958902E-2</v>
+      </c>
+      <c r="G30" s="1">
+        <v>16</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0.21917808219178</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="1">
+        <v>97</v>
+      </c>
+      <c r="C31" s="1">
+        <v>74</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.76288659793814395</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1">
+        <v>23</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0.23711340206185499</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="1">
+        <v>531</v>
+      </c>
+      <c r="C32" s="1">
+        <v>369</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.69491525423728795</v>
+      </c>
+      <c r="E32" s="1">
+        <v>83</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0.15630885122410501</v>
+      </c>
+      <c r="G32" s="1">
+        <v>79</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0.14877589453860601</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="1">
+        <v>138</v>
+      </c>
+      <c r="C33" s="1">
+        <v>77</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0.55797101449275299</v>
+      </c>
+      <c r="E33" s="1">
+        <v>31</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0.22463768115942001</v>
+      </c>
+      <c r="G33" s="1">
+        <v>30</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0.217391304347826</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="1">
+        <v>655</v>
+      </c>
+      <c r="C34" s="1">
+        <v>401</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0.61221374045801502</v>
+      </c>
+      <c r="E34" s="1">
+        <v>147</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0.22442748091602999</v>
+      </c>
+      <c r="G34" s="1">
+        <v>107</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0.16335877862595399</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1">
+        <v>776</v>
+      </c>
+      <c r="C35" s="1">
+        <v>555</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.71520618556700999</v>
+      </c>
+      <c r="E35" s="1">
+        <v>129</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0.16623711340206099</v>
+      </c>
+      <c r="G35" s="1">
+        <v>92</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0.118556701030927</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="1">
+        <v>29</v>
+      </c>
+      <c r="C36" s="1">
+        <v>23</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0.79310344827586199</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1">
+        <v>6</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0.20689655172413701</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="1">
+        <v>28</v>
+      </c>
+      <c r="C37" s="1">
+        <v>19</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.67857142857142805</v>
+      </c>
+      <c r="E37" s="1">
+        <v>6</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0.214285714285714</v>
+      </c>
+      <c r="G37" s="1">
+        <v>3</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0.107142857142857</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="1">
+        <v>16</v>
+      </c>
+      <c r="C38" s="1">
+        <v>10</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="E38" s="1">
+        <v>3</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0.1875</v>
+      </c>
+      <c r="G38" s="1">
+        <v>3</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="1">
+        <v>14</v>
+      </c>
+      <c r="C39" s="1">
+        <v>8</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0.57142857142857095</v>
+      </c>
+      <c r="E39" s="1">
+        <v>3</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0.214285714285714</v>
+      </c>
+      <c r="G39" s="1">
+        <v>3</v>
+      </c>
+      <c r="H39" s="1">
+        <v>0.214285714285714</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="1">
+        <v>186</v>
+      </c>
+      <c r="C40" s="1">
+        <v>120</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0.64516129032257996</v>
+      </c>
+      <c r="E40" s="1">
+        <v>38</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0.204301075268817</v>
+      </c>
+      <c r="G40" s="1">
+        <v>28</v>
+      </c>
+      <c r="H40" s="1">
+        <v>0.15053763440860199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="1">
+        <v>175</v>
+      </c>
+      <c r="C41" s="1">
+        <v>76</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0.434285714285714</v>
+      </c>
+      <c r="E41" s="1">
+        <v>73</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0.41714285714285698</v>
+      </c>
+      <c r="G41" s="1">
+        <v>26</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0.14857142857142799</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="1">
+        <v>54</v>
+      </c>
+      <c r="C42" s="1">
+        <v>14</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0.25925925925925902</v>
+      </c>
+      <c r="E42" s="1">
+        <v>38</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0.70370370370370305</v>
+      </c>
+      <c r="G42" s="1">
+        <v>2</v>
+      </c>
+      <c r="H42" s="1">
+        <v>3.7037037037037E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" s="1">
+        <v>526</v>
+      </c>
+      <c r="C43" s="1">
+        <v>443</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0.84220532319391594</v>
+      </c>
+      <c r="E43" s="1">
+        <v>53</v>
+      </c>
+      <c r="F43" s="1">
+        <v>0.100760456273764</v>
+      </c>
+      <c r="G43" s="1">
+        <v>30</v>
+      </c>
+      <c r="H43" s="1">
+        <v>5.7034220532319303E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" s="1">
+        <v>451</v>
+      </c>
+      <c r="C44" s="1">
+        <v>325</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0.72062084257206205</v>
+      </c>
+      <c r="E44" s="1">
+        <v>95</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0.21064301552106399</v>
+      </c>
+      <c r="G44" s="1">
+        <v>31</v>
+      </c>
+      <c r="H44" s="1">
+        <v>6.8736141906873605E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" s="1">
+        <v>102</v>
+      </c>
+      <c r="C45" s="1">
+        <v>68</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="E45" s="1">
+        <v>15</v>
+      </c>
+      <c r="F45" s="1">
+        <v>0.14705882352941099</v>
+      </c>
+      <c r="G45" s="1">
+        <v>19</v>
+      </c>
+      <c r="H45" s="1">
+        <v>0.18627450980392099</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="1">
+        <v>213</v>
+      </c>
+      <c r="C46" s="1">
+        <v>126</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0.59154929577464699</v>
+      </c>
+      <c r="E46" s="1">
+        <v>62</v>
+      </c>
+      <c r="F46" s="1">
+        <v>0.29107981220657198</v>
+      </c>
+      <c r="G46" s="1">
+        <v>25</v>
+      </c>
+      <c r="H46" s="1">
+        <v>0.117370892018779</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="1">
+        <v>120</v>
+      </c>
+      <c r="C47" s="1">
+        <v>90</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="E47" s="1">
+        <v>13</v>
+      </c>
+      <c r="F47" s="1">
+        <v>0.108333333333333</v>
+      </c>
+      <c r="G47" s="1">
+        <v>17</v>
+      </c>
+      <c r="H47" s="1">
+        <v>0.141666666666666</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" s="1">
+        <v>85</v>
+      </c>
+      <c r="C48" s="1">
+        <v>54</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0.63529411764705801</v>
+      </c>
+      <c r="E48" s="1">
+        <v>13</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0.152941176470588</v>
+      </c>
+      <c r="G48" s="1">
+        <v>18</v>
+      </c>
+      <c r="H48" s="1">
+        <v>0.21176470588235199</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B49" s="1">
+        <v>136</v>
+      </c>
+      <c r="C49" s="1">
+        <v>92</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0.67647058823529405</v>
+      </c>
+      <c r="E49" s="1">
+        <v>23</v>
+      </c>
+      <c r="F49" s="1">
+        <v>0.16911764705882301</v>
+      </c>
+      <c r="G49" s="1">
+        <v>21</v>
+      </c>
+      <c r="H49" s="1">
+        <v>0.154411764705882</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B50" s="1">
+        <v>204</v>
+      </c>
+      <c r="C50" s="1">
+        <v>169</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0.828431372549019</v>
+      </c>
+      <c r="E50" s="1">
+        <v>17</v>
+      </c>
+      <c r="F50" s="1">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="G50" s="1">
+        <v>18</v>
+      </c>
+      <c r="H50" s="1">
+        <v>8.8235294117646995E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B51" s="1">
+        <v>15</v>
+      </c>
+      <c r="C51" s="1">
+        <v>6</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E51" s="1">
+        <v>6</v>
+      </c>
+      <c r="F51" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="G51" s="1">
+        <v>3</v>
+      </c>
+      <c r="H51" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52" s="1">
+        <v>54</v>
+      </c>
+      <c r="C52" s="1">
+        <v>36</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <v>0</v>
+      </c>
+      <c r="G52" s="1">
+        <v>18</v>
+      </c>
+      <c r="H52" s="1">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" s="1">
+        <v>58</v>
+      </c>
+      <c r="C53" s="1">
+        <v>46</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0.79310344827586199</v>
+      </c>
+      <c r="E53" s="1">
+        <v>4</v>
+      </c>
+      <c r="F53" s="1">
+        <v>6.8965517241379296E-2</v>
+      </c>
+      <c r="G53" s="1">
+        <v>8</v>
+      </c>
+      <c r="H53" s="1">
+        <v>0.13793103448275801</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55" s="1">
+        <v>4779</v>
+      </c>
+      <c r="C55" s="1">
+        <v>3277</v>
+      </c>
+      <c r="D55" s="1">
+        <v>0.68570830717723297</v>
+      </c>
+      <c r="E55" s="1">
+        <v>867</v>
+      </c>
+      <c r="F55" s="1">
+        <v>0.181418706842435</v>
+      </c>
+      <c r="G55" s="1">
+        <v>635</v>
+      </c>
+      <c r="H55" s="1">
+        <v>0.13287298598033001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>